<commit_message>
atualização com dados mais recentes do dataframe
</commit_message>
<xml_diff>
--- a/dataframe.xlsx
+++ b/dataframe.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/399fcb3130b8647a/tcc/maquina vetor suporte/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luc-g\Desktop\SVR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{E4370003-6880-4D4D-9580-F8126C3D1FE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9A2A182-C790-4409-989F-7336443C2A30}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93ABEC87-E0DE-4F80-A2F1-C5E72F28FF2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{64909D5C-DD0E-4957-BD5C-497FEF4F3194}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{64909D5C-DD0E-4957-BD5C-497FEF4F3194}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -134,7 +134,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -156,6 +156,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -470,20 +476,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6F285A8-2E86-4D1B-AAA2-BD3C7791E40D}">
-  <dimension ref="A1:E202"/>
+  <dimension ref="A1:E204"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B209" sqref="B209"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="28.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5546875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="28.6640625" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -500,7 +506,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>39448</v>
       </c>
@@ -517,7 +523,7 @@
         <v>3783.8651166163795</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>39479</v>
       </c>
@@ -534,7 +540,7 @@
         <v>3793.1293949021397</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>39508</v>
       </c>
@@ -551,7 +557,7 @@
         <v>3807.9781082910004</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>39539</v>
       </c>
@@ -568,7 +574,7 @@
         <v>3835.305131185783</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>39569</v>
       </c>
@@ -585,7 +591,7 @@
         <v>3866.5345736870145</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>39600</v>
       </c>
@@ -602,7 +608,7 @@
         <v>3901.3347700728359</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>39630</v>
       </c>
@@ -619,7 +625,7 @@
         <v>3919.17788535311</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>39661</v>
       </c>
@@ -636,7 +642,7 @@
         <v>3944.0236832364722</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>39692</v>
       </c>
@@ -653,7 +659,7 @@
         <v>3983.9371245187544</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>39722</v>
       </c>
@@ -670,7 +676,7 @@
         <v>4043.4270415557444</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>39753</v>
       </c>
@@ -687,7 +693,7 @@
         <v>4095.2796994361788</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>39783</v>
       </c>
@@ -704,7 +710,7 @@
         <v>4145.1785315286506</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>39814</v>
       </c>
@@ -721,7 +727,7 @@
         <v>4173.618619666262</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>39845</v>
       </c>
@@ -738,7 +744,7 @@
         <v>4209.1703812501692</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>39873</v>
       </c>
@@ -755,7 +761,7 @@
         <v>4245.4628746983817</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>39904</v>
       </c>
@@ -772,7 +778,7 @@
         <v>4285.2889564241113</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>39934</v>
       </c>
@@ -789,7 +795,7 @@
         <v>4332.8408833542471</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>39965</v>
       </c>
@@ -806,7 +812,7 @@
         <v>4372.7368872696652</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>39995</v>
       </c>
@@ -823,7 +829,7 @@
         <v>4446.0180485676037</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>40026</v>
       </c>
@@ -840,7 +846,7 @@
         <v>4523.0159764930459</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>40057</v>
       </c>
@@ -857,7 +863,7 @@
         <v>4614.6869343600438</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>40087</v>
       </c>
@@ -874,7 +880,7 @@
         <v>4703.3187162190952</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>40118</v>
       </c>
@@ -891,7 +897,7 @@
         <v>4793.1735811251701</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>40148</v>
       </c>
@@ -908,7 +914,7 @@
         <v>4882.4540872693624</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>40179</v>
       </c>
@@ -925,7 +931,7 @@
         <v>4983.0028034311399</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>40210</v>
       </c>
@@ -942,7 +948,7 @@
         <v>5094.220085541474</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>40238</v>
       </c>
@@ -959,7 +965,7 @@
         <v>5197.9380540572256</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>40269</v>
       </c>
@@ -976,7 +982,7 @@
         <v>5303.2755537485591</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>40299</v>
       </c>
@@ -993,7 +999,7 @@
         <v>5403.1158453146945</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>40330</v>
       </c>
@@ -1010,7 +1016,7 @@
         <v>5513.8965458702496</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>40360</v>
       </c>
@@ -1027,7 +1033,7 @@
         <v>5639.0611305116672</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>40391</v>
       </c>
@@ -1044,7 +1050,7 @@
         <v>5787.589958085121</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>40422</v>
       </c>
@@ -1061,7 +1067,7 @@
         <v>5958.6856218231042</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>40452</v>
       </c>
@@ -1078,7 +1084,7 @@
         <v>6117.7943846287535</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>40483</v>
       </c>
@@ -1095,7 +1101,7 @@
         <v>6284.3619208254695</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>40513</v>
       </c>
@@ -1112,7 +1118,7 @@
         <v>6447.5509149024529</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>40544</v>
       </c>
@@ -1129,7 +1135,7 @@
         <v>6614.3510796957808</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>40575</v>
       </c>
@@ -1146,7 +1152,7 @@
         <v>6796.7012268349217</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>40603</v>
       </c>
@@ -1163,7 +1169,7 @@
         <v>7012.9589404668495</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>40634</v>
       </c>
@@ -1180,7 +1186,7 @@
         <v>7233.5021644790513</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>40664</v>
       </c>
@@ -1197,7 +1203,7 @@
         <v>7468.8385758375325</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>40695</v>
       </c>
@@ -1214,7 +1220,7 @@
         <v>7701.0723718720201</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>40725</v>
       </c>
@@ -1231,7 +1237,7 @@
         <v>7927.9508181091078</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <v>40756</v>
       </c>
@@ -1248,7 +1254,7 @@
         <v>8211.83701723177</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>40787</v>
       </c>
@@ -1265,7 +1271,7 @@
         <v>8572.7194269519241</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
         <v>40817</v>
       </c>
@@ -1282,7 +1288,7 @@
         <v>8864.4527001302013</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>40848</v>
       </c>
@@ -1299,7 +1305,7 @@
         <v>8932.7737460374083</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
         <v>40878</v>
       </c>
@@ -1316,7 +1322,7 @@
         <v>8946.1498206581473</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>40909</v>
       </c>
@@ -1333,7 +1339,7 @@
         <v>9000.0691540378266</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
         <v>40940</v>
       </c>
@@ -1350,7 +1356,7 @@
         <v>9217.8568738252143</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>40969</v>
       </c>
@@ -1367,7 +1373,7 @@
         <v>9415.6053042968906</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
         <v>41000</v>
       </c>
@@ -1384,7 +1390,7 @@
         <v>9665.5968125758482</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>41030</v>
       </c>
@@ -1401,7 +1407,7 @@
         <v>9799.0842956391389</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
         <v>41061</v>
       </c>
@@ -1418,7 +1424,7 @@
         <v>9864.3513291718591</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>41091</v>
       </c>
@@ -1435,7 +1441,7 @@
         <v>9922.3613493838166</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="3">
         <v>41122</v>
       </c>
@@ -1452,7 +1458,7 @@
         <v>10015.461757576186</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>41153</v>
       </c>
@@ -1469,7 +1475,7 @@
         <v>10114.775221909895</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
         <v>41183</v>
       </c>
@@ -1486,7 +1492,7 @@
         <v>10192.568250707958</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>41214</v>
       </c>
@@ -1503,7 +1509,7 @@
         <v>10317.839438925259</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="3">
         <v>41244</v>
       </c>
@@ -1520,7 +1526,7 @@
         <v>10471.427268416539</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <v>41275</v>
       </c>
@@ -1537,7 +1543,7 @@
         <v>10589.326617261944</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="3">
         <v>41306</v>
       </c>
@@ -1554,7 +1560,7 @@
         <v>10705.693167621988</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <v>41334</v>
       </c>
@@ -1571,7 +1577,7 @@
         <v>10820.034686690633</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="3">
         <v>41365</v>
       </c>
@@ -1588,7 +1594,7 @@
         <v>10946.537297674122</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <v>41395</v>
       </c>
@@ -1605,7 +1611,7 @@
         <v>11048.41829581081</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="3">
         <v>41426</v>
       </c>
@@ -1622,7 +1628,7 @@
         <v>11149.339675591256</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <v>41456</v>
       </c>
@@ -1639,7 +1645,7 @@
         <v>11227.419484153288</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="3">
         <v>41487</v>
       </c>
@@ -1656,7 +1662,7 @@
         <v>11292.317577933494</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
         <v>41518</v>
       </c>
@@ -1673,7 +1679,7 @@
         <v>11344.001731139508</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="3">
         <v>41548</v>
       </c>
@@ -1690,7 +1696,7 @@
         <v>11380.52909458063</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="2">
         <v>41579</v>
       </c>
@@ -1707,7 +1713,7 @@
         <v>11471.166196812163</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="3">
         <v>41609</v>
       </c>
@@ -1724,7 +1730,7 @@
         <v>11552.092789657207</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="2">
         <v>41640</v>
       </c>
@@ -1741,7 +1747,7 @@
         <v>11641.326712197289</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="3">
         <v>41671</v>
       </c>
@@ -1758,7 +1764,7 @@
         <v>11722.750748861323</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="2">
         <v>41699</v>
       </c>
@@ -1775,7 +1781,7 @@
         <v>11807.22652768005</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="3">
         <v>41730</v>
       </c>
@@ -1792,7 +1798,7 @@
         <v>11882.011049460543</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="2">
         <v>41760</v>
       </c>
@@ -1809,7 +1815,7 @@
         <v>11932.677120021232</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="3">
         <v>41791</v>
       </c>
@@ -1826,7 +1832,7 @@
         <v>11964.179939951413</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" s="2">
         <v>41821</v>
       </c>
@@ -1843,7 +1849,7 @@
         <v>11997.184851469987</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="3">
         <v>41852</v>
       </c>
@@ -1860,7 +1866,7 @@
         <v>12032.819779107562</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" s="2">
         <v>41883</v>
       </c>
@@ -1877,7 +1883,7 @@
         <v>12074.433136214499</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" s="3">
         <v>41913</v>
       </c>
@@ -1894,7 +1900,7 @@
         <v>12115.318004951903</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="2">
         <v>41944</v>
       </c>
@@ -1911,7 +1917,7 @@
         <v>12151.391161180143</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="3">
         <v>41974</v>
       </c>
@@ -1928,7 +1934,7 @@
         <v>12159.184021342895</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" s="2">
         <v>42005</v>
       </c>
@@ -1945,7 +1951,7 @@
         <v>12184.285626667192</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" s="3">
         <v>42036</v>
       </c>
@@ -1962,7 +1968,7 @@
         <v>12201.970368507082</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" s="2">
         <v>42064</v>
       </c>
@@ -1979,7 +1985,7 @@
         <v>12271.614933312976</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" s="3">
         <v>42095</v>
       </c>
@@ -1996,7 +2002,7 @@
         <v>12320.64972278061</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" s="2">
         <v>42125</v>
       </c>
@@ -2013,7 +2019,7 @@
         <v>12365.916967357933</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" s="3">
         <v>42156</v>
       </c>
@@ -2030,7 +2036,7 @@
         <v>12371.566022622119</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" s="2">
         <v>42186</v>
       </c>
@@ -2047,7 +2053,7 @@
         <v>12359.54507759168</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" s="3">
         <v>42217</v>
       </c>
@@ -2064,7 +2070,7 @@
         <v>12317.768442782517</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" s="2">
         <v>42248</v>
       </c>
@@ -2081,7 +2087,7 @@
         <v>12285.58738980443</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" s="3">
         <v>42278</v>
       </c>
@@ -2098,7 +2104,7 @@
         <v>12236.074140655481</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" s="2">
         <v>42309</v>
       </c>
@@ -2115,7 +2121,7 @@
         <v>12189.542253425452</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" s="3">
         <v>42339</v>
       </c>
@@ -2132,7 +2138,7 @@
         <v>12134.994517235034</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" s="2">
         <v>42370</v>
       </c>
@@ -2149,7 +2155,7 @@
         <v>12125.831369203224</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" s="3">
         <v>42401</v>
       </c>
@@ -2166,7 +2172,7 @@
         <v>12117.563982486314</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" s="2">
         <v>42430</v>
       </c>
@@ -2183,7 +2189,7 @@
         <v>12123.522147692684</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" s="3">
         <v>42461</v>
       </c>
@@ -2200,7 +2206,7 @@
         <v>12114.889533191177</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" s="2">
         <v>42491</v>
       </c>
@@ -2217,7 +2223,7 @@
         <v>12110.36404313717</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" s="3">
         <v>42522</v>
       </c>
@@ -2234,7 +2240,7 @@
         <v>12108.4477247635</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" s="2">
         <v>42552</v>
       </c>
@@ -2251,7 +2257,7 @@
         <v>12103.368231413508</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" s="3">
         <v>42583</v>
       </c>
@@ -2268,7 +2274,7 @@
         <v>12100.039518563757</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" s="2">
         <v>42614</v>
       </c>
@@ -2285,7 +2291,7 @@
         <v>12112.130495038098</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" s="3">
         <v>42644</v>
       </c>
@@ -2302,7 +2308,7 @@
         <v>12126.202053325051</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" s="2">
         <v>42675</v>
       </c>
@@ -2319,7 +2325,7 @@
         <v>12137.034634250629</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" s="3">
         <v>42705</v>
       </c>
@@ -2336,7 +2342,7 @@
         <v>12149.34713866653</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" s="2">
         <v>42736</v>
       </c>
@@ -2353,7 +2359,7 @@
         <v>12157.440081184584</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" s="3">
         <v>42767</v>
       </c>
@@ -2370,7 +2376,7 @@
         <v>12168.000999225584</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" s="2">
         <v>42795</v>
       </c>
@@ -2387,7 +2393,7 @@
         <v>12131.271605316133</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" s="3">
         <v>42826</v>
       </c>
@@ -2404,7 +2410,7 @@
         <v>12094.307217459551</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" s="2">
         <v>42856</v>
       </c>
@@ -2421,7 +2427,7 @@
         <v>12024.793835950562</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" s="3">
         <v>42887</v>
       </c>
@@ -2438,7 +2444,7 @@
         <v>11995.532173870521</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" s="2">
         <v>42917</v>
       </c>
@@ -2455,7 +2461,7 @@
         <v>11944.036240363248</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" s="3">
         <v>42948</v>
       </c>
@@ -2472,7 +2478,7 @@
         <v>11919.227266831815</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" s="2">
         <v>42979</v>
       </c>
@@ -2489,7 +2495,7 @@
         <v>11870.426741740634</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" s="3">
         <v>43009</v>
       </c>
@@ -2506,7 +2512,7 @@
         <v>11898.396821413227</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" s="2">
         <v>43040</v>
       </c>
@@ -2523,7 +2529,7 @@
         <v>11911.589684761682</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" s="3">
         <v>43070</v>
       </c>
@@ -2540,7 +2546,7 @@
         <v>11947.049609968359</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" s="2">
         <v>43101</v>
       </c>
@@ -2557,7 +2563,7 @@
         <v>11908.868228722016</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" s="3">
         <v>43132</v>
       </c>
@@ -2574,7 +2580,7 @@
         <v>11897.894928780308</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" s="2">
         <v>43160</v>
       </c>
@@ -2591,7 +2597,7 @@
         <v>11864.092193787845</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" s="3">
         <v>43191</v>
       </c>
@@ -2608,7 +2614,7 @@
         <v>11845.573246424976</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" s="2">
         <v>43221</v>
       </c>
@@ -2625,7 +2631,7 @@
         <v>11816.779471093729</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" s="3">
         <v>43252</v>
       </c>
@@ -2642,7 +2648,7 @@
         <v>11780.777941581871</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" s="2">
         <v>43282</v>
       </c>
@@ -2659,7 +2665,7 @@
         <v>11755.095912896584</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" s="3">
         <v>43313</v>
       </c>
@@ -2676,7 +2682,7 @@
         <v>11709.981492779971</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" s="2">
         <v>43344</v>
       </c>
@@ -2693,7 +2699,7 @@
         <v>11665.962933789842</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" s="3">
         <v>43374</v>
       </c>
@@ -2710,7 +2716,7 @@
         <v>11623.658625402575</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" s="2">
         <v>43405</v>
       </c>
@@ -2727,7 +2733,7 @@
         <v>11596.83108955997</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" s="3">
         <v>43435</v>
       </c>
@@ -2744,7 +2750,7 @@
         <v>11605.44832876299</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" s="2">
         <v>43466</v>
       </c>
@@ -2761,7 +2767,7 @@
         <v>11636.225670304662</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" s="3">
         <v>43497</v>
       </c>
@@ -2778,7 +2784,7 @@
         <v>11645.368500964123</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" s="2">
         <v>43525</v>
       </c>
@@ -2795,7 +2801,7 @@
         <v>11626.037919259283</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" s="3">
         <v>43556</v>
       </c>
@@ -2812,7 +2818,7 @@
         <v>11581.231908840442</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" s="2">
         <v>43586</v>
       </c>
@@ -2829,7 +2835,7 @@
         <v>11545.651022848266</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" s="3">
         <v>43617</v>
       </c>
@@ -2846,7 +2852,7 @@
         <v>11512.87040304575</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" s="2">
         <v>43647</v>
       </c>
@@ -2863,7 +2869,7 @@
         <v>11488.550902769906</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" s="3">
         <v>43678</v>
       </c>
@@ -2880,7 +2886,7 @@
         <v>11458.912056293555</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" s="2">
         <v>43709</v>
       </c>
@@ -2897,7 +2903,7 @@
         <v>11422.180421137058</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" s="3">
         <v>43739</v>
       </c>
@@ -2914,7 +2920,7 @@
         <v>11406.904087812274</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" s="2">
         <v>43770</v>
       </c>
@@ -2931,7 +2937,7 @@
         <v>11387.423817199868</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" s="3">
         <v>43800</v>
       </c>
@@ -2948,7 +2954,7 @@
         <v>11376.282005699379</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" s="2">
         <v>43831</v>
       </c>
@@ -2965,7 +2971,7 @@
         <v>11375.676492220349</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" s="3">
         <v>43862</v>
       </c>
@@ -2982,7 +2988,7 @@
         <v>11370.318078795932</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" s="2">
         <v>43891</v>
       </c>
@@ -2999,7 +3005,7 @@
         <v>11338.417310958648</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" s="3">
         <v>43922</v>
       </c>
@@ -3016,7 +3022,7 @@
         <v>11317.99595492375</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" s="2">
         <v>43952</v>
       </c>
@@ -3033,7 +3039,7 @@
         <v>11291.761478764369</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" s="3">
         <v>43983</v>
       </c>
@@ -3050,7 +3056,7 @@
         <v>11319.346699763859</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" s="2">
         <v>44013</v>
       </c>
@@ -3067,7 +3073,7 @@
         <v>11364.729566501239</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" s="3">
         <v>44044</v>
       </c>
@@ -3084,7 +3090,7 @@
         <v>11408.060328611698</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" s="2">
         <v>44075</v>
       </c>
@@ -3101,7 +3107,7 @@
         <v>11445.023688686617</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" s="3">
         <v>44105</v>
       </c>
@@ -3118,7 +3124,7 @@
         <v>11470.408303037939</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" s="2">
         <v>44136</v>
       </c>
@@ -3135,7 +3141,7 @@
         <v>11513.864891737097</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157" s="3">
         <v>44166</v>
       </c>
@@ -3152,7 +3158,7 @@
         <v>11567.058455041313</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" s="2">
         <v>44197</v>
       </c>
@@ -3169,7 +3175,7 @@
         <v>11634.299214640889</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159" s="3">
         <v>44228</v>
       </c>
@@ -3186,7 +3192,7 @@
         <v>11722.617812364795</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160" s="2">
         <v>44256</v>
       </c>
@@ -3203,7 +3209,7 @@
         <v>11767.787957031309</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161" s="3">
         <v>44287</v>
       </c>
@@ -3220,7 +3226,7 @@
         <v>11795.872223523293</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162" s="2">
         <v>44317</v>
       </c>
@@ -3237,7 +3243,7 @@
         <v>11810.193645590163</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163" s="3">
         <v>44348</v>
       </c>
@@ -3254,7 +3260,7 @@
         <v>11832.289128402614</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164" s="2">
         <v>44378</v>
       </c>
@@ -3271,7 +3277,7 @@
         <v>11880.365296326469</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165" s="3">
         <v>44409</v>
       </c>
@@ -3288,7 +3294,7 @@
         <v>11930.744394366713</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" s="2">
         <v>44440</v>
       </c>
@@ -3305,7 +3311,7 @@
         <v>11990.080997296634</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" s="3">
         <v>44470</v>
       </c>
@@ -3322,7 +3328,7 @@
         <v>12038.021987233904</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" s="2">
         <v>44501</v>
       </c>
@@ -3339,7 +3345,7 @@
         <v>12076.054714831891</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169" s="3">
         <v>44531</v>
       </c>
@@ -3356,7 +3362,7 @@
         <v>12121.074040642643</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170" s="2">
         <v>44562</v>
       </c>
@@ -3373,7 +3379,7 @@
         <v>12141.683049875874</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171" s="3">
         <v>44593</v>
       </c>
@@ -3390,7 +3396,7 @@
         <v>12166.943266726179</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172" s="2">
         <v>44621</v>
       </c>
@@ -3407,7 +3413,7 @@
         <v>12184.505791338703</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A173" s="3">
         <v>44652</v>
       </c>
@@ -3424,7 +3430,7 @@
         <v>12237.059628945724</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174" s="2">
         <v>44682</v>
       </c>
@@ -3441,7 +3447,7 @@
         <v>12277.098353468662</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175" s="3">
         <v>44713</v>
       </c>
@@ -3458,7 +3464,7 @@
         <v>12312.396668497795</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176" s="2">
         <v>44743</v>
       </c>
@@ -3475,7 +3481,7 @@
         <v>12327.407825425218</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177" s="3">
         <v>44774</v>
       </c>
@@ -3492,7 +3498,7 @@
         <v>12367.180957715922</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178" s="2">
         <v>44805</v>
       </c>
@@ -3509,7 +3515,7 @@
         <v>12429.564298412692</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179" s="3">
         <v>44835</v>
       </c>
@@ -3526,7 +3532,7 @@
         <v>12460.344710476546</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180" s="2">
         <v>44866</v>
       </c>
@@ -3543,7 +3549,7 @@
         <v>12451.096748009519</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A181" s="3">
         <v>44896</v>
       </c>
@@ -3560,7 +3566,7 @@
         <v>12445.556467509607</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A182" s="2">
         <v>44927</v>
       </c>
@@ -3577,7 +3583,7 @@
         <v>12461.878128178887</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183" s="3">
         <v>44958</v>
       </c>
@@ -3594,7 +3600,7 @@
         <v>12489.704163074459</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184" s="2">
         <v>44986</v>
       </c>
@@ -3611,7 +3617,7 @@
         <v>12490.278667365916</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A185" s="3">
         <v>45017</v>
       </c>
@@ -3628,7 +3634,7 @@
         <v>12495.515451059071</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186" s="2">
         <v>45047</v>
       </c>
@@ -3645,7 +3651,7 @@
         <v>12505.118173155639</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187" s="3">
         <v>45078</v>
       </c>
@@ -3662,7 +3668,7 @@
         <v>12521.040247201072</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188" s="2">
         <v>45108</v>
       </c>
@@ -3679,7 +3685,7 @@
         <v>12562.900617701647</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A189" s="3">
         <v>45139</v>
       </c>
@@ -3696,7 +3702,7 @@
         <v>12600.146604093594</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190" s="2">
         <v>45170</v>
       </c>
@@ -3713,7 +3719,7 @@
         <v>12637.294678384957</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A191" s="3">
         <v>45200</v>
       </c>
@@ -3730,7 +3736,7 @@
         <v>12638.726953524943</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A192" s="2">
         <v>45231</v>
       </c>
@@ -3747,7 +3753,7 @@
         <v>12647.765385086304</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A193" s="3">
         <v>45261</v>
       </c>
@@ -3764,7 +3770,7 @@
         <v>12643.18080370294</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A194" s="2">
         <v>45292</v>
       </c>
@@ -3781,7 +3787,7 @@
         <v>12635.764481282376</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A195" s="3">
         <v>45323</v>
       </c>
@@ -3798,7 +3804,7 @@
         <v>12596.219823390687</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A196" s="2">
         <v>45352</v>
       </c>
@@ -3815,7 +3821,7 @@
         <v>12584.699175456704</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A197" s="3">
         <v>45383</v>
       </c>
@@ -3832,7 +3838,7 @@
         <v>12574.667926565247</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A198" s="2">
         <v>45413</v>
       </c>
@@ -3849,7 +3855,7 @@
         <v>12607.13895025622</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A199" s="3">
         <v>45444</v>
       </c>
@@ -3866,7 +3872,7 @@
         <v>12596.993075676362</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A200" s="2">
         <v>45474</v>
       </c>
@@ -3883,7 +3889,7 @@
         <v>12613.741323152777</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A201" s="3">
         <v>45505</v>
       </c>
@@ -3900,7 +3906,7 @@
         <v>12632.766041903318</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A202" s="2">
         <v>45536</v>
       </c>
@@ -3915,6 +3921,40 @@
       </c>
       <c r="E202" s="6">
         <v>12683.128392060196</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A203" s="3">
+        <v>45566</v>
+      </c>
+      <c r="B203" s="10">
+        <v>12211.965621494297</v>
+      </c>
+      <c r="C203" s="10">
+        <v>8753.6079830345188</v>
+      </c>
+      <c r="D203" s="10">
+        <v>10139.293052175881</v>
+      </c>
+      <c r="E203" s="10">
+        <v>12713.760123937198</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A204" s="2">
+        <v>45597</v>
+      </c>
+      <c r="B204" s="9">
+        <v>12270.129890606033</v>
+      </c>
+      <c r="C204" s="9">
+        <v>8760.7592709400124</v>
+      </c>
+      <c r="D204" s="9">
+        <v>10161.471674378226</v>
+      </c>
+      <c r="E204" s="9">
+        <v>12726.053897725724</v>
       </c>
     </row>
   </sheetData>

</xml_diff>